<commit_message>
Cadastro de Ingredientes - Index
</commit_message>
<xml_diff>
--- a/Tabela_TACO_2011.xlsx
+++ b/Tabela_TACO_2011.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\BakeryManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\BakeryManager\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3567" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="630">
   <si>
     <t>Colesterol</t>
   </si>
@@ -1191,9 +1191,6 @@
   </si>
   <si>
     <t>Carne, bovina, paleta, com gordura, crua</t>
-  </si>
-  <si>
-    <t>,0,02</t>
   </si>
   <si>
     <t>Carne, bovina, paleta, sem gordura, cozida</t>
@@ -2691,7 +2688,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB598"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C573" workbookViewId="0">
+      <selection activeCell="Z376" sqref="Z376"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2701,25 +2700,25 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C1" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1" t="s">
         <v>615</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>616</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>617</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>619</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
@@ -2728,31 +2727,31 @@
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>623</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>624</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>625</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>626</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>3</v>
@@ -2767,7 +2766,7 @@
         <v>6</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>7</v>
@@ -2782,7 +2781,7 @@
         <v>10</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -4163,7 +4162,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -33173,8 +33172,8 @@
       <c r="Y374">
         <v>0.04</v>
       </c>
-      <c r="Z374" t="s">
-        <v>389</v>
+      <c r="Z374">
+        <v>0.02</v>
       </c>
       <c r="AA374">
         <v>0.91</v>
@@ -33185,7 +33184,7 @@
         <v>374</v>
       </c>
       <c r="B375" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C375">
         <v>62.9</v>
@@ -33268,7 +33267,7 @@
         <v>375</v>
       </c>
       <c r="B376" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C376">
         <v>72.099999999999994</v>
@@ -33351,7 +33350,7 @@
         <v>376</v>
       </c>
       <c r="B377" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C377">
         <v>72.900000000000006</v>
@@ -33434,7 +33433,7 @@
         <v>377</v>
       </c>
       <c r="B378" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C378">
         <v>55.2</v>
@@ -33517,7 +33516,7 @@
         <v>378</v>
       </c>
       <c r="B379" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C379">
         <v>51.2</v>
@@ -33600,7 +33599,7 @@
         <v>379</v>
       </c>
       <c r="B380" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C380">
         <v>61.5</v>
@@ -33683,7 +33682,7 @@
         <v>380</v>
       </c>
       <c r="B381" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C381">
         <v>65.599999999999994</v>
@@ -33766,7 +33765,7 @@
         <v>381</v>
       </c>
       <c r="B382" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C382">
         <v>53.4</v>
@@ -33849,7 +33848,7 @@
         <v>382</v>
       </c>
       <c r="B383" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C383">
         <v>72.400000000000006</v>
@@ -33932,7 +33931,7 @@
         <v>383</v>
       </c>
       <c r="B384" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C384">
         <v>54.6</v>
@@ -34015,7 +34014,7 @@
         <v>384</v>
       </c>
       <c r="B385" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C385">
         <v>47.2</v>
@@ -34098,7 +34097,7 @@
         <v>385</v>
       </c>
       <c r="B386" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C386">
         <v>39.200000000000003</v>
@@ -34181,7 +34180,7 @@
         <v>386</v>
       </c>
       <c r="B387" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C387">
         <v>42.2</v>
@@ -34261,7 +34260,7 @@
         <v>387</v>
       </c>
       <c r="B388" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C388">
         <v>56</v>
@@ -34338,7 +34337,7 @@
         <v>388</v>
       </c>
       <c r="B389" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C389">
         <v>39.200000000000003</v>
@@ -34415,7 +34414,7 @@
         <v>389</v>
       </c>
       <c r="B390" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C390">
         <v>28.2</v>
@@ -34495,7 +34494,7 @@
         <v>390</v>
       </c>
       <c r="B391" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C391">
         <v>32</v>
@@ -34575,7 +34574,7 @@
         <v>391</v>
       </c>
       <c r="B392" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C392">
         <v>67.5</v>
@@ -34658,7 +34657,7 @@
         <v>392</v>
       </c>
       <c r="B393" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C393">
         <v>59.7</v>
@@ -34741,7 +34740,7 @@
         <v>393</v>
       </c>
       <c r="B394" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C394">
         <v>61.4</v>
@@ -34824,7 +34823,7 @@
         <v>394</v>
       </c>
       <c r="B395" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C395">
         <v>69.099999999999994</v>
@@ -34907,7 +34906,7 @@
         <v>395</v>
       </c>
       <c r="B396" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C396">
         <v>63.5</v>
@@ -34990,7 +34989,7 @@
         <v>396</v>
       </c>
       <c r="B397" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C397">
         <v>59.8</v>
@@ -35073,7 +35072,7 @@
         <v>397</v>
       </c>
       <c r="B398" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C398">
         <v>72.900000000000006</v>
@@ -35156,7 +35155,7 @@
         <v>398</v>
       </c>
       <c r="B399" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C399">
         <v>66.7</v>
@@ -35239,7 +35238,7 @@
         <v>399</v>
       </c>
       <c r="B400" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C400">
         <v>76.400000000000006</v>
@@ -35322,7 +35321,7 @@
         <v>400</v>
       </c>
       <c r="B401" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C401">
         <v>77.8</v>
@@ -35405,7 +35404,7 @@
         <v>401</v>
       </c>
       <c r="B402" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C402">
         <v>54.9</v>
@@ -35488,7 +35487,7 @@
         <v>402</v>
       </c>
       <c r="B403" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C403">
         <v>66.5</v>
@@ -35571,7 +35570,7 @@
         <v>403</v>
       </c>
       <c r="B404" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C404">
         <v>63.2</v>
@@ -35654,7 +35653,7 @@
         <v>404</v>
       </c>
       <c r="B405" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C405">
         <v>67.5</v>
@@ -35737,7 +35736,7 @@
         <v>405</v>
       </c>
       <c r="B406" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C406">
         <v>74.900000000000006</v>
@@ -35820,7 +35819,7 @@
         <v>406</v>
       </c>
       <c r="B407" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C407">
         <v>58.5</v>
@@ -35903,7 +35902,7 @@
         <v>407</v>
       </c>
       <c r="B408" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C408">
         <v>71.900000000000006</v>
@@ -35986,7 +35985,7 @@
         <v>408</v>
       </c>
       <c r="B409" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C409">
         <v>65.599999999999994</v>
@@ -36069,7 +36068,7 @@
         <v>409</v>
       </c>
       <c r="B410" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C410">
         <v>74.8</v>
@@ -36152,7 +36151,7 @@
         <v>410</v>
       </c>
       <c r="B411" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C411">
         <v>63.8</v>
@@ -36235,7 +36234,7 @@
         <v>411</v>
       </c>
       <c r="B412" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C412">
         <v>55</v>
@@ -36318,7 +36317,7 @@
         <v>412</v>
       </c>
       <c r="B413" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C413">
         <v>63.6</v>
@@ -36401,7 +36400,7 @@
         <v>413</v>
       </c>
       <c r="B414" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C414">
         <v>55.6</v>
@@ -36484,7 +36483,7 @@
         <v>414</v>
       </c>
       <c r="B415" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C415">
         <v>72.7</v>
@@ -36567,7 +36566,7 @@
         <v>415</v>
       </c>
       <c r="B416" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C416">
         <v>63.6</v>
@@ -36644,7 +36643,7 @@
         <v>416</v>
       </c>
       <c r="B417" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C417">
         <v>52.5</v>
@@ -36721,7 +36720,7 @@
         <v>417</v>
       </c>
       <c r="B418" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C418">
         <v>59.2</v>
@@ -36798,7 +36797,7 @@
         <v>418</v>
       </c>
       <c r="B419" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C419">
         <v>64.8</v>
@@ -36875,7 +36874,7 @@
         <v>419</v>
       </c>
       <c r="B420" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C420">
         <v>59.6</v>
@@ -36952,7 +36951,7 @@
         <v>420</v>
       </c>
       <c r="B421" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C421">
         <v>58.6</v>
@@ -37029,7 +37028,7 @@
         <v>421</v>
       </c>
       <c r="B422" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C422">
         <v>62.5</v>
@@ -37106,7 +37105,7 @@
         <v>422</v>
       </c>
       <c r="B423" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C423">
         <v>54.6</v>
@@ -37183,7 +37182,7 @@
         <v>423</v>
       </c>
       <c r="B424" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C424">
         <v>50.5</v>
@@ -37260,7 +37259,7 @@
         <v>424</v>
       </c>
       <c r="B425" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C425">
         <v>56.4</v>
@@ -37337,7 +37336,7 @@
         <v>425</v>
       </c>
       <c r="B426" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C426">
         <v>65.3</v>
@@ -37420,7 +37419,7 @@
         <v>426</v>
       </c>
       <c r="B427" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C427">
         <v>78.2</v>
@@ -37503,7 +37502,7 @@
         <v>427</v>
       </c>
       <c r="B428" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C428">
         <v>67.7</v>
@@ -37586,7 +37585,7 @@
         <v>428</v>
       </c>
       <c r="B429" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C429">
         <v>47.3</v>
@@ -37669,7 +37668,7 @@
         <v>429</v>
       </c>
       <c r="B430" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C430">
         <v>51.8</v>
@@ -37752,7 +37751,7 @@
         <v>430</v>
       </c>
       <c r="B431" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C431">
         <v>36.9</v>
@@ -37835,7 +37834,7 @@
         <v>431</v>
       </c>
       <c r="B432" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C432">
         <v>61.2</v>
@@ -37918,7 +37917,7 @@
         <v>432</v>
       </c>
       <c r="B433" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C433">
         <v>56.6</v>
@@ -38001,7 +38000,7 @@
         <v>433</v>
       </c>
       <c r="B434" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C434">
         <v>67.7</v>
@@ -38084,7 +38083,7 @@
         <v>434</v>
       </c>
       <c r="B435" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C435">
         <v>59.7</v>
@@ -38167,7 +38166,7 @@
         <v>435</v>
       </c>
       <c r="B436" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C436">
         <v>49.3</v>
@@ -38250,7 +38249,7 @@
         <v>436</v>
       </c>
       <c r="B437" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C437">
         <v>67.099999999999994</v>
@@ -38333,7 +38332,7 @@
         <v>437</v>
       </c>
       <c r="B438" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C438">
         <v>43.8</v>
@@ -38416,7 +38415,7 @@
         <v>438</v>
       </c>
       <c r="B439" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C439">
         <v>73.900000000000006</v>
@@ -38499,7 +38498,7 @@
         <v>439</v>
       </c>
       <c r="B440" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C440">
         <v>77.2</v>
@@ -38582,7 +38581,7 @@
         <v>440</v>
       </c>
       <c r="B441" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C441">
         <v>69</v>
@@ -38662,7 +38661,7 @@
         <v>441</v>
       </c>
       <c r="B442" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C442">
         <v>74.5</v>
@@ -38742,7 +38741,7 @@
         <v>442</v>
       </c>
       <c r="B443" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C443">
         <v>54</v>
@@ -38819,7 +38818,7 @@
         <v>443</v>
       </c>
       <c r="B444" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C444">
         <v>34.700000000000003</v>
@@ -38896,7 +38895,7 @@
         <v>444</v>
       </c>
       <c r="B445" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C445">
         <v>27.6</v>
@@ -38979,7 +38978,7 @@
         <v>445</v>
       </c>
       <c r="B446" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C446">
         <v>6.3</v>
@@ -39062,7 +39061,7 @@
         <v>446</v>
       </c>
       <c r="B447" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C447">
         <v>87.7</v>
@@ -39142,7 +39141,7 @@
         <v>447</v>
       </c>
       <c r="B448" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C448">
         <v>70.900000000000006</v>
@@ -39222,7 +39221,7 @@
         <v>448</v>
       </c>
       <c r="B449" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C449">
         <v>90</v>
@@ -39302,7 +39301,7 @@
         <v>449</v>
       </c>
       <c r="B450" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C450">
         <v>89.2</v>
@@ -39382,7 +39381,7 @@
         <v>450</v>
       </c>
       <c r="B451" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C451" t="s">
         <v>97</v>
@@ -39459,7 +39458,7 @@
         <v>451</v>
       </c>
       <c r="B452" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C452">
         <v>84.6</v>
@@ -39539,7 +39538,7 @@
         <v>452</v>
       </c>
       <c r="B453" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C453">
         <v>85.1</v>
@@ -39619,7 +39618,7 @@
         <v>453</v>
       </c>
       <c r="B454" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C454">
         <v>27</v>
@@ -39699,7 +39698,7 @@
         <v>454</v>
       </c>
       <c r="B455" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C455">
         <v>87.1</v>
@@ -39779,7 +39778,7 @@
         <v>455</v>
       </c>
       <c r="B456" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C456">
         <v>80.900000000000006</v>
@@ -39859,7 +39858,7 @@
         <v>456</v>
       </c>
       <c r="B457" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C457">
         <v>3.1</v>
@@ -39936,7 +39935,7 @@
         <v>457</v>
       </c>
       <c r="B458" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C458" t="s">
         <v>97</v>
@@ -40016,7 +40015,7 @@
         <v>458</v>
       </c>
       <c r="B459" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C459" t="s">
         <v>97</v>
@@ -40096,7 +40095,7 @@
         <v>459</v>
       </c>
       <c r="B460" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C460">
         <v>2.7</v>
@@ -40176,7 +40175,7 @@
         <v>460</v>
       </c>
       <c r="B461" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C461">
         <v>81.900000000000006</v>
@@ -40256,7 +40255,7 @@
         <v>461</v>
       </c>
       <c r="B462" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C462">
         <v>56.1</v>
@@ -40336,7 +40335,7 @@
         <v>462</v>
       </c>
       <c r="B463" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C463">
         <v>47.1</v>
@@ -40413,7 +40412,7 @@
         <v>463</v>
       </c>
       <c r="B464" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C464">
         <v>45.3</v>
@@ -40490,7 +40489,7 @@
         <v>464</v>
       </c>
       <c r="B465" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C465">
         <v>21.2</v>
@@ -40570,7 +40569,7 @@
         <v>465</v>
       </c>
       <c r="B466" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C466">
         <v>54.4</v>
@@ -40650,7 +40649,7 @@
         <v>466</v>
       </c>
       <c r="B467" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C467">
         <v>72.2</v>
@@ -40730,7 +40729,7 @@
         <v>467</v>
       </c>
       <c r="B468" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C468">
         <v>42.4</v>
@@ -40807,7 +40806,7 @@
         <v>468</v>
       </c>
       <c r="B469" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C469">
         <v>62.5</v>
@@ -40887,7 +40886,7 @@
         <v>469</v>
       </c>
       <c r="B470" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C470">
         <v>73.599999999999994</v>
@@ -40967,7 +40966,7 @@
         <v>470</v>
       </c>
       <c r="B471" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C471">
         <v>93.5</v>
@@ -41032,7 +41031,7 @@
         <v>471</v>
       </c>
       <c r="B472" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C472">
         <v>97.4</v>
@@ -41097,7 +41096,7 @@
         <v>472</v>
       </c>
       <c r="B473" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D473">
         <v>216</v>
@@ -41159,7 +41158,7 @@
         <v>473</v>
       </c>
       <c r="B474" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C474">
         <v>81.7</v>
@@ -41239,7 +41238,7 @@
         <v>474</v>
       </c>
       <c r="B475" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C475">
         <v>92.4</v>
@@ -41319,7 +41318,7 @@
         <v>475</v>
       </c>
       <c r="B476" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C476">
         <v>99.6</v>
@@ -41399,7 +41398,7 @@
         <v>476</v>
       </c>
       <c r="B477" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C477">
         <v>99.3</v>
@@ -41479,7 +41478,7 @@
         <v>477</v>
       </c>
       <c r="B478" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C478">
         <v>99.4</v>
@@ -41559,7 +41558,7 @@
         <v>478</v>
       </c>
       <c r="B479" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C479">
         <v>94.3</v>
@@ -41639,7 +41638,7 @@
         <v>479</v>
       </c>
       <c r="B480" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C480">
         <v>92</v>
@@ -41704,7 +41703,7 @@
         <v>480</v>
       </c>
       <c r="B481" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C481">
         <v>91.3</v>
@@ -41769,7 +41768,7 @@
         <v>481</v>
       </c>
       <c r="B482" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C482">
         <v>90</v>
@@ -41834,7 +41833,7 @@
         <v>482</v>
       </c>
       <c r="B483" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C483">
         <v>88.2</v>
@@ -41899,7 +41898,7 @@
         <v>483</v>
       </c>
       <c r="B484" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C484">
         <v>89.7</v>
@@ -41964,7 +41963,7 @@
         <v>484</v>
       </c>
       <c r="B485" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C485">
         <v>60.5</v>
@@ -42044,7 +42043,7 @@
         <v>485</v>
       </c>
       <c r="B486" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C486">
         <v>71.7</v>
@@ -42124,7 +42123,7 @@
         <v>486</v>
       </c>
       <c r="B487" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C487">
         <v>85.2</v>
@@ -42204,7 +42203,7 @@
         <v>487</v>
       </c>
       <c r="B488" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C488">
         <v>50</v>
@@ -42284,7 +42283,7 @@
         <v>488</v>
       </c>
       <c r="B489" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C489">
         <v>75.8</v>
@@ -42364,7 +42363,7 @@
         <v>489</v>
       </c>
       <c r="B490" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C490">
         <v>75.599999999999994</v>
@@ -42444,7 +42443,7 @@
         <v>490</v>
       </c>
       <c r="B491" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C491">
         <v>63.5</v>
@@ -42524,7 +42523,7 @@
         <v>491</v>
       </c>
       <c r="B492" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C492">
         <v>1.1000000000000001</v>
@@ -42604,7 +42603,7 @@
         <v>492</v>
       </c>
       <c r="B493" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C493">
         <v>0.1</v>
@@ -42655,7 +42654,7 @@
         <v>3</v>
       </c>
       <c r="S493" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="T493" t="s">
         <v>14</v>
@@ -42669,7 +42668,7 @@
         <v>493</v>
       </c>
       <c r="B494" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C494">
         <v>3.3</v>
@@ -42749,7 +42748,7 @@
         <v>494</v>
       </c>
       <c r="B495" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C495">
         <v>0.1</v>
@@ -42800,7 +42799,7 @@
         <v>6</v>
       </c>
       <c r="S495" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="T495" t="s">
         <v>14</v>
@@ -42814,7 +42813,7 @@
         <v>495</v>
       </c>
       <c r="B496" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C496">
         <v>1.3</v>
@@ -42900,7 +42899,7 @@
         <v>496</v>
       </c>
       <c r="B497" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C497">
         <v>1.2</v>
@@ -42980,7 +42979,7 @@
         <v>497</v>
       </c>
       <c r="B498" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C498">
         <v>1.7</v>
@@ -43060,7 +43059,7 @@
         <v>498</v>
       </c>
       <c r="B499" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C499">
         <v>1</v>
@@ -43140,7 +43139,7 @@
         <v>499</v>
       </c>
       <c r="B500" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C500">
         <v>3.4</v>
@@ -43220,7 +43219,7 @@
         <v>500</v>
       </c>
       <c r="B501" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C501">
         <v>43.9</v>
@@ -43300,7 +43299,7 @@
         <v>501</v>
       </c>
       <c r="B502" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C502">
         <v>27.5</v>
@@ -43386,7 +43385,7 @@
         <v>502</v>
       </c>
       <c r="B503" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C503">
         <v>73.5</v>
@@ -43472,7 +43471,7 @@
         <v>503</v>
       </c>
       <c r="B504" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C504">
         <v>20.399999999999999</v>
@@ -43552,7 +43551,7 @@
         <v>504</v>
       </c>
       <c r="B505" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C505">
         <v>21.6</v>
@@ -43632,7 +43631,7 @@
         <v>505</v>
       </c>
       <c r="B506" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C506">
         <v>20.7</v>
@@ -43712,7 +43711,7 @@
         <v>506</v>
       </c>
       <c r="B507" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C507">
         <v>28.5</v>
@@ -43792,7 +43791,7 @@
         <v>507</v>
       </c>
       <c r="B508" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C508">
         <v>15.8</v>
@@ -43872,7 +43871,7 @@
         <v>508</v>
       </c>
       <c r="B509" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C509">
         <v>22.1</v>
@@ -43952,7 +43951,7 @@
         <v>509</v>
       </c>
       <c r="B510" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C510">
         <v>23.9</v>
@@ -44032,7 +44031,7 @@
         <v>510</v>
       </c>
       <c r="B511" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C511">
         <v>7.1</v>
@@ -44112,7 +44111,7 @@
         <v>511</v>
       </c>
       <c r="B512" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C512">
         <v>2.9</v>
@@ -44192,7 +44191,7 @@
         <v>512</v>
       </c>
       <c r="B513" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C513">
         <v>2.6</v>
@@ -44272,7 +44271,7 @@
         <v>513</v>
       </c>
       <c r="B514" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C514">
         <v>7.1</v>
@@ -44352,7 +44351,7 @@
         <v>514</v>
       </c>
       <c r="B515" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C515">
         <v>71.900000000000006</v>
@@ -44432,7 +44431,7 @@
         <v>515</v>
       </c>
       <c r="B516" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C516">
         <v>1.2</v>
@@ -44512,7 +44511,7 @@
         <v>516</v>
       </c>
       <c r="B517" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C517">
         <v>0.6</v>
@@ -44556,7 +44555,7 @@
         <v>517</v>
       </c>
       <c r="B518" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C518">
         <v>0.4</v>
@@ -44594,7 +44593,7 @@
         <v>518</v>
       </c>
       <c r="B519" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C519">
         <v>70.599999999999994</v>
@@ -44674,7 +44673,7 @@
         <v>519</v>
       </c>
       <c r="B520" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C520">
         <v>7.7</v>
@@ -44715,7 +44714,7 @@
         <v>520</v>
       </c>
       <c r="B521" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C521">
         <v>68.5</v>
@@ -44795,7 +44794,7 @@
         <v>521</v>
       </c>
       <c r="B522" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C522">
         <v>76.3</v>
@@ -44875,7 +44874,7 @@
         <v>522</v>
       </c>
       <c r="B523" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C523">
         <v>55.1</v>
@@ -44958,7 +44957,7 @@
         <v>523</v>
       </c>
       <c r="B524" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C524">
         <v>78</v>
@@ -45038,7 +45037,7 @@
         <v>524</v>
       </c>
       <c r="B525" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C525">
         <v>58.4</v>
@@ -45118,7 +45117,7 @@
         <v>525</v>
       </c>
       <c r="B526" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C526">
         <v>50.5</v>
@@ -45198,7 +45197,7 @@
         <v>526</v>
       </c>
       <c r="B527" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C527">
         <v>68</v>
@@ -45278,7 +45277,7 @@
         <v>527</v>
       </c>
       <c r="B528" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C528">
         <v>69.099999999999994</v>
@@ -45358,7 +45357,7 @@
         <v>528</v>
       </c>
       <c r="B529" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C529">
         <v>71.2</v>
@@ -45438,7 +45437,7 @@
         <v>529</v>
       </c>
       <c r="B530" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C530">
         <v>54.2</v>
@@ -45515,7 +45514,7 @@
         <v>530</v>
       </c>
       <c r="B531" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C531">
         <v>41.5</v>
@@ -45595,7 +45594,7 @@
         <v>531</v>
       </c>
       <c r="B532" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C532">
         <v>82</v>
@@ -45675,7 +45674,7 @@
         <v>532</v>
       </c>
       <c r="B533" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C533">
         <v>81.5</v>
@@ -45755,7 +45754,7 @@
         <v>533</v>
       </c>
       <c r="B534" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C534">
         <v>71.099999999999994</v>
@@ -45835,7 +45834,7 @@
         <v>534</v>
       </c>
       <c r="B535" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C535">
         <v>68.900000000000006</v>
@@ -45915,7 +45914,7 @@
         <v>535</v>
       </c>
       <c r="B536" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C536">
         <v>81</v>
@@ -46001,7 +46000,7 @@
         <v>536</v>
       </c>
       <c r="B537" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C537">
         <v>75.3</v>
@@ -46081,7 +46080,7 @@
         <v>537</v>
       </c>
       <c r="B538" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C538">
         <v>70.099999999999994</v>
@@ -46158,7 +46157,7 @@
         <v>538</v>
       </c>
       <c r="B539" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C539">
         <v>70.900000000000006</v>
@@ -46235,7 +46234,7 @@
         <v>539</v>
       </c>
       <c r="B540" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C540">
         <v>61.7</v>
@@ -46315,7 +46314,7 @@
         <v>540</v>
       </c>
       <c r="B541" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C541">
         <v>71.8</v>
@@ -46401,7 +46400,7 @@
         <v>541</v>
       </c>
       <c r="B542" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C542">
         <v>79.5</v>
@@ -46481,7 +46480,7 @@
         <v>542</v>
       </c>
       <c r="B543" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C543">
         <v>71.400000000000006</v>
@@ -46561,7 +46560,7 @@
         <v>543</v>
       </c>
       <c r="B544" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C544">
         <v>76.400000000000006</v>
@@ -46647,7 +46646,7 @@
         <v>544</v>
       </c>
       <c r="B545" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C545">
         <v>81.099999999999994</v>
@@ -46730,7 +46729,7 @@
         <v>545</v>
       </c>
       <c r="B546" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C546">
         <v>82</v>
@@ -46816,7 +46815,7 @@
         <v>546</v>
       </c>
       <c r="B547" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C547">
         <v>90</v>
@@ -46902,7 +46901,7 @@
         <v>547</v>
       </c>
       <c r="B548" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C548">
         <v>72.5</v>
@@ -46988,7 +46987,7 @@
         <v>548</v>
       </c>
       <c r="B549" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C549">
         <v>75</v>
@@ -47065,7 +47064,7 @@
         <v>549</v>
       </c>
       <c r="B550" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C550">
         <v>85.8</v>
@@ -47145,7 +47144,7 @@
         <v>550</v>
       </c>
       <c r="B551" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C551">
         <v>85.2</v>
@@ -47228,7 +47227,7 @@
         <v>551</v>
       </c>
       <c r="B552" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C552">
         <v>24.9</v>
@@ -47308,7 +47307,7 @@
         <v>552</v>
       </c>
       <c r="B553" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C553">
         <v>91.9</v>
@@ -47394,7 +47393,7 @@
         <v>553</v>
       </c>
       <c r="B554" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C554">
         <v>75</v>
@@ -47474,7 +47473,7 @@
         <v>554</v>
       </c>
       <c r="B555" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C555">
         <v>58.4</v>
@@ -47554,7 +47553,7 @@
         <v>555</v>
       </c>
       <c r="B556" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C556">
         <v>48.6</v>
@@ -47634,7 +47633,7 @@
         <v>556</v>
       </c>
       <c r="B557" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C557">
         <v>69.400000000000006</v>
@@ -47720,7 +47719,7 @@
         <v>557</v>
       </c>
       <c r="B558" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C558">
         <v>6.4</v>
@@ -47800,7 +47799,7 @@
         <v>558</v>
       </c>
       <c r="B559" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C559">
         <v>1.7</v>
@@ -47880,7 +47879,7 @@
         <v>559</v>
       </c>
       <c r="B560" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C560">
         <v>76.8</v>
@@ -47960,7 +47959,7 @@
         <v>560</v>
       </c>
       <c r="B561" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C561">
         <v>80.099999999999994</v>
@@ -48046,7 +48045,7 @@
         <v>561</v>
       </c>
       <c r="B562" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C562">
         <v>80.400000000000006</v>
@@ -48126,7 +48125,7 @@
         <v>562</v>
       </c>
       <c r="B563" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C563">
         <v>14</v>
@@ -48206,7 +48205,7 @@
         <v>563</v>
       </c>
       <c r="B564" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C564">
         <v>80</v>
@@ -48286,7 +48285,7 @@
         <v>564</v>
       </c>
       <c r="B565" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C565">
         <v>12.7</v>
@@ -48366,7 +48365,7 @@
         <v>565</v>
       </c>
       <c r="B566" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C566">
         <v>75.8</v>
@@ -48446,7 +48445,7 @@
         <v>566</v>
       </c>
       <c r="B567" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C567">
         <v>13.5</v>
@@ -48526,7 +48525,7 @@
         <v>567</v>
       </c>
       <c r="B568" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C568">
         <v>80.2</v>
@@ -48606,7 +48605,7 @@
         <v>568</v>
       </c>
       <c r="B569" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C569">
         <v>14.9</v>
@@ -48686,7 +48685,7 @@
         <v>569</v>
       </c>
       <c r="B570" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C570">
         <v>77.900000000000006</v>
@@ -48766,7 +48765,7 @@
         <v>570</v>
       </c>
       <c r="B571" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C571">
         <v>15</v>
@@ -48846,7 +48845,7 @@
         <v>571</v>
       </c>
       <c r="B572" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C572">
         <v>82.6</v>
@@ -48926,7 +48925,7 @@
         <v>572</v>
       </c>
       <c r="B573" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C573">
         <v>12</v>
@@ -49006,7 +49005,7 @@
         <v>573</v>
       </c>
       <c r="B574" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C574">
         <v>80</v>
@@ -49086,7 +49085,7 @@
         <v>574</v>
       </c>
       <c r="B575" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C575">
         <v>12.6</v>
@@ -49166,7 +49165,7 @@
         <v>575</v>
       </c>
       <c r="B576" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C576">
         <v>12.3</v>
@@ -49246,7 +49245,7 @@
         <v>576</v>
       </c>
       <c r="B577" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C577">
         <v>11.4</v>
@@ -49326,7 +49325,7 @@
         <v>577</v>
       </c>
       <c r="B578" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C578">
         <v>76.3</v>
@@ -49406,7 +49405,7 @@
         <v>578</v>
       </c>
       <c r="B579" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C579">
         <v>11.5</v>
@@ -49492,7 +49491,7 @@
         <v>579</v>
       </c>
       <c r="B580" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C580">
         <v>1.8</v>
@@ -49572,7 +49571,7 @@
         <v>580</v>
       </c>
       <c r="B581" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C581">
         <v>2.9</v>
@@ -49652,7 +49651,7 @@
         <v>581</v>
       </c>
       <c r="B582" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C582">
         <v>5.8</v>
@@ -49732,7 +49731,7 @@
         <v>582</v>
       </c>
       <c r="B583" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C583">
         <v>91.3</v>
@@ -49812,7 +49811,7 @@
         <v>583</v>
       </c>
       <c r="B584" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C584">
         <v>4.5</v>
@@ -49892,7 +49891,7 @@
         <v>584</v>
       </c>
       <c r="B585" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C585">
         <v>86.6</v>
@@ -49972,7 +49971,7 @@
         <v>585</v>
       </c>
       <c r="B586" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C586">
         <v>9.6999999999999993</v>
@@ -50052,7 +50051,7 @@
         <v>586</v>
       </c>
       <c r="B587" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C587">
         <v>67.7</v>
@@ -50132,7 +50131,7 @@
         <v>587</v>
       </c>
       <c r="B588" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C588">
         <v>3.1</v>
@@ -50212,7 +50211,7 @@
         <v>588</v>
       </c>
       <c r="B589" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C589">
         <v>3.5</v>
@@ -50292,7 +50291,7 @@
         <v>589</v>
       </c>
       <c r="B590" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C590">
         <v>3.5</v>
@@ -50372,7 +50371,7 @@
         <v>590</v>
       </c>
       <c r="B591" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C591">
         <v>43</v>
@@ -50452,7 +50451,7 @@
         <v>591</v>
       </c>
       <c r="B592" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C592" t="s">
         <v>97</v>
@@ -50532,7 +50531,7 @@
         <v>592</v>
       </c>
       <c r="B593" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C593">
         <v>15.8</v>
@@ -50612,7 +50611,7 @@
         <v>593</v>
       </c>
       <c r="B594" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C594">
         <v>3.9</v>
@@ -50692,7 +50691,7 @@
         <v>594</v>
       </c>
       <c r="B595" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C595">
         <v>6.7</v>
@@ -50772,7 +50771,7 @@
         <v>595</v>
       </c>
       <c r="B596" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C596">
         <v>50.5</v>
@@ -50852,7 +50851,7 @@
         <v>596</v>
       </c>
       <c r="B597" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C597">
         <v>54.5</v>
@@ -50938,7 +50937,7 @@
         <v>597</v>
       </c>
       <c r="B598" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C598">
         <v>6.2</v>

</xml_diff>